<commit_message>
Update PROBAST and extraction
</commit_message>
<xml_diff>
--- a/Systematic_review/Extraction_PAI_studies_final_CM_KH_CM.xlsx
+++ b/Systematic_review/Extraction_PAI_studies_final_CM_KH_CM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meinkcha.PSYCHOLOGIE\Documents\GitHub\PAI_paper_analysis_new\Systematic_review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C2B647-ED7E-4C13-8C60-D090E1DD8293}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C528632-A021-4E43-8CC2-C8A4B89B02D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="10310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="10310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study_characteristics_table" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="198">
   <si>
     <t>depression</t>
   </si>
@@ -271,9 +271,6 @@
     <t>Sample size</t>
   </si>
   <si>
-    <t>Diagnosis</t>
-  </si>
-  <si>
     <t>Treatment options</t>
   </si>
   <si>
@@ -329,10 +326,6 @@
 PCL-5: 4.69</t>
   </si>
   <si>
-    <t xml:space="preserve"> CAPS-5: 0.55
-PCL-5: 0.47</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.93 </t>
   </si>
   <si>
@@ -489,10 +482,6 @@
     <t>FBB-ADHS, FBB-SSV</t>
   </si>
   <si>
-    <t>ADHD: d = 0.35
-ODD: d = 0.54</t>
-  </si>
-  <si>
     <t>veterans with PTSD</t>
   </si>
   <si>
@@ -514,25 +503,6 @@
     <t>DBT  vs. GPM</t>
   </si>
   <si>
-    <t xml:space="preserve">Blended-treatment - Face2Face CBT with internet-based CBT elements
-CBT - Cognitive Behavioral Therapy
-CBT - EE - Cognitive Behaviorale Therapy with integrated exposure and emotion-focused elements
-CFD - Person-centered counselling for depression
-DBT - dialectical behavior therapy
-EMDR - Eye movement desensitization and reprocessing
-Encert - CBT enriched with emotion regulation training
-GPM - general psychiatric management
-iPE - intensified Prolongued Exposure
-IPPI-D - Integrative Positive Psychological Intervention for Depression
-IPT - Interpersonal Psychotherapy
-PDT - Psychodynamic Therapy
-PE - Prolongued Exposure
-STAIR - skills training
-TAU - Treatment as usual
-Tf-CBT - Trauma-focused Cognitive Behavioral Therapy
-</t>
-  </si>
-  <si>
     <t>GSI SQL</t>
   </si>
   <si>
@@ -542,17 +512,10 @@
     <t>random forest  recursive partitioning (“mobforest”) and subsequent bootstrapped backward selection  (“bootstepAIC”)</t>
   </si>
   <si>
-    <t>linear regression (? No info in the paper)</t>
-  </si>
-  <si>
     <t>(1000 *) 10-fold</t>
   </si>
   <si>
     <t>baseline GSI symptom severity, childhood emotional abuse (CTQ), dependent personality traits (IPDE), impulsivity BPD symptoms (Zanarini scale), social adjustment (SAS), and depression (BDI)</t>
-  </si>
-  <si>
-    <t>initial model: d = 0.36
-less biased model: d = 0.22</t>
   </si>
   <si>
     <t>Keefe et al., 2021</t>
@@ -689,6 +652,56 @@
   <si>
     <t>ADHD symptoms: ADHD, ODD
 ODD symptoms: ODD, functional impairment, single parenthood</t>
+  </si>
+  <si>
+    <t>ADHD: 0.35
+ODD: 0.54</t>
+  </si>
+  <si>
+    <t>initial model: 0.36
+less biased model: 0.22</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>0.37</t>
+  </si>
+  <si>
+    <t>0.21</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>CAPS-5: 0.55
+PCL-5: 0.47</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>Diagnosis / Target Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blended-treatment - Face2Face CBT with internet-based CBT elements
+CBT - Cognitive Behavioral Therapy
+CBT - EE - Cognitive Behaviorale Therapy with integrated exposure and emotion-focused elements
+CFD - Person-centered counselling for depression
+CT - Cognitive Therapy
+DBT - dialectical behavior therapy
+EMDR - Eye movement desensitization and reprocessing
+Encert - CBT enriched with emotion regulation training
+GPM - general psychiatric management
+iPE - intensified Prolongued Exposure
+IPPI-D - Integrative Positive Psychological Intervention for Depression
+IPT - Interpersonal Psychotherapy
+PDT - Psychodynamic Therapy
+PE - Prolongued Exposure
+STAIR - skills training
+TAU - Treatment as usual
+Tf-CBT - Trauma-focused Cognitive Behavioral Therapy
+</t>
   </si>
 </sst>
 </file>
@@ -847,6 +860,33 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -950,11 +990,16 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
         <top/>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -971,14 +1016,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -990,30 +1027,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1057,16 +1070,16 @@
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{26BC8255-5CCB-4F34-86AD-633D2050EE4E}" name="First Author, Year"/>
     <tableColumn id="2" xr3:uid="{FBCC4217-93B8-4D52-8CCF-7C65CF1ED1F9}" name="Sample size" totalsRowFunction="sum"/>
-    <tableColumn id="3" xr3:uid="{FA191619-4393-4AB3-A475-F1CFB18FBFAD}" name="Diagnosis"/>
+    <tableColumn id="3" xr3:uid="{FA191619-4393-4AB3-A475-F1CFB18FBFAD}" name="Diagnosis / Target Group"/>
     <tableColumn id="4" xr3:uid="{0DDE27D7-1B9B-4962-ABEE-70F25ADEA78E}" name="Treatment options"/>
     <tableColumn id="5" xr3:uid="{0766634A-3F86-434E-A411-18AB705A3FF3}" name="Post-treatment severity measure"/>
-    <tableColumn id="6" xr3:uid="{64321D5F-9077-4744-974B-7372092EAD76}" name="Type of feature selection approach" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{64321D5F-9077-4744-974B-7372092EAD76}" name="Type of feature selection approach" dataDxfId="20" totalsRowDxfId="3"/>
     <tableColumn id="7" xr3:uid="{E33915D8-CFE2-436F-A9BF-5D9E5BA5CB37}" name="Type of outcome prediction approach"/>
     <tableColumn id="8" xr3:uid="{C8F11DA9-E46B-4A3C-A2EA-43C623B0E195}" name="CV scheme"/>
     <tableColumn id="9" xr3:uid="{AF59ABE1-EFC9-4F1A-A96D-4DFB71EE9CC3}" name="Most relevant predictors"/>
-    <tableColumn id="10" xr3:uid="{535BD486-F558-40E0-9FB2-CFDFDB9AB6B9}" name="Mean absolute PAI" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{ADAFFF80-3039-44A0-8021-B6FB044E14E3}" name="Mean diff in post-treatment severity (optimal vs. non-optimal)" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{D713BB7A-0E11-4EBC-8332-F9F20E34689C}" name="Cohen's d for optimal vs non-optimal" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{535BD486-F558-40E0-9FB2-CFDFDB9AB6B9}" name="Mean absolute PAI" dataDxfId="19" totalsRowDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{ADAFFF80-3039-44A0-8021-B6FB044E14E3}" name="Mean diff in post-treatment severity (optimal vs. non-optimal)" dataDxfId="18" totalsRowDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{D713BB7A-0E11-4EBC-8332-F9F20E34689C}" name="Cohen's d for optimal vs non-optimal" dataDxfId="17" totalsRowDxfId="0"/>
     <tableColumn id="13" xr3:uid="{2B04E87D-4E65-41C0-AA5C-551C4AA30D44}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1074,22 +1087,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:J27" totalsRowCount="1" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:J27" totalsRowCount="1" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:J26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:J26">
-    <sortCondition ref="D1:D26"/>
-  </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="First Author, Year" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Mean absolute PAI" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Mean diff in post-treatment severity (optimal vs. non-optimal)" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Cohen's d for optimal vs non-optimal" totalsRowFunction="average" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="First Author, Year" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Mean absolute PAI" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Mean diff in post-treatment severity (optimal vs. non-optimal)" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Cohen's d for optimal vs non-optimal" totalsRowFunction="average" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{B352E868-CEC6-434E-B11D-83740571B00E}" name="Cohen´s d significant?"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Subsample: definition" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Subsample: Mean absolute PAI " dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Subsample:Mean diff in post-treatment severity between optimal vs. non-optimal2" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Subsample: Cohen's d for optimal vs non-optimal" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{F54836A1-CCDD-44DD-97EE-114310B8C16C}" name="Subsample: Cohen´s d significant?" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Subsample: definition" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Subsample: Mean absolute PAI " dataDxfId="9"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Subsample:Mean diff in post-treatment severity between optimal vs. non-optimal2" dataDxfId="8"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Subsample: Cohen's d for optimal vs non-optimal" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{F54836A1-CCDD-44DD-97EE-114310B8C16C}" name="Subsample: Cohen´s d significant?" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1099,7 +1109,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4887E5A3-67DC-4346-AFF2-63EF760CB90D}" name="Tabelle2" displayName="Tabelle2" ref="A1:I4" totalsRowShown="0">
   <autoFilter ref="A1:I4" xr:uid="{4887E5A3-67DC-4346-AFF2-63EF760CB90D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{DB374AE6-D1A9-4866-A600-2508D7CF8601}" name="Study" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{DB374AE6-D1A9-4866-A600-2508D7CF8601}" name="Study" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{45CB4E32-4B95-4664-ACBD-4FE904FAF87A}" name="mean_optimal"/>
     <tableColumn id="3" xr3:uid="{8998A52E-BF7E-4A7B-8E14-8872430EA111}" name="SD_optimal"/>
     <tableColumn id="4" xr3:uid="{7768716D-6E16-47FA-B193-A1C2FC88D988}" name="mean_nonoptimal"/>
@@ -1110,7 +1120,7 @@
     <tableColumn id="7" xr3:uid="{29CFBB65-1916-4045-8A23-87704C7C9E58}" name="Pooled SD">
       <calculatedColumnFormula xml:space="preserve"> SQRT((Tabelle2[[#This Row],[SD_optimal]]^2+Tabelle2[[#This Row],[SD_nonoptimal]]^2)/2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{13D2015A-3158-43F8-9845-88E0A358319F}" name="Cohen´s d" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{13D2015A-3158-43F8-9845-88E0A358319F}" name="Cohen´s d" dataDxfId="4">
       <calculatedColumnFormula>ROUND(Tabelle2[[#This Row],[Difference_means]]/Tabelle2[[#This Row],[Pooled SD]],2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{A65AA7CA-4450-4870-9557-705489AA9375}" name="Assumptions"/>
@@ -1384,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02586865-404A-4994-BBC5-FA512A75A132}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="A24" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1413,209 +1423,209 @@
         <v>77</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="159" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="6">
-        <v>200</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="L2" s="17">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2">
+        <v>996</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>137</v>
       </c>
       <c r="B3">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>24</v>
+        <v>139</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>166</v>
       </c>
       <c r="G3" t="s">
         <v>40</v>
       </c>
-      <c r="H3" t="s">
-        <v>93</v>
-      </c>
-      <c r="I3" t="s">
-        <v>109</v>
+      <c r="H3" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>164</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="K3" s="13">
-        <v>1.6</v>
-      </c>
-      <c r="L3" s="13">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K3" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="159" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="6">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>110</v>
+        <v>20</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="K4" s="12">
-        <v>3.03</v>
-      </c>
-      <c r="L4" s="12">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>46</v>
+        <v>23</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="I5" t="s">
-        <v>111</v>
-      </c>
-      <c r="J5" s="13">
-        <v>4.2</v>
+        <v>107</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="K5" s="13">
-        <v>1.78</v>
+        <v>1.6</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>103</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="6">
-        <v>123</v>
+        <v>225</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>40</v>
@@ -1624,74 +1634,74 @@
         <v>27</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="K6" s="12">
-        <v>1.35</v>
+        <v>3.03</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7">
-        <v>245</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H7" t="s">
         <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>70</v>
+        <v>195</v>
       </c>
       <c r="K7" s="13">
-        <v>2.33</v>
+        <v>1.78</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="B8" s="6">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>74</v>
+        <v>4</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>40</v>
@@ -1700,481 +1710,481 @@
         <v>27</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="6">
-        <v>134</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="K8" s="12">
+        <v>1.35</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>245</v>
+      </c>
+      <c r="C9" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="J9" s="12">
-        <v>8.9</v>
-      </c>
-      <c r="K9" s="12">
-        <v>6</v>
-      </c>
-      <c r="L9" s="12">
-        <v>0.51</v>
+      <c r="I9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" s="13">
+        <v>2.33</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10">
-        <v>262</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
+        <v>145</v>
+      </c>
+      <c r="B10" s="23">
+        <v>110</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>186</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>147</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>48</v>
+        <v>169</v>
       </c>
       <c r="G10" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="25" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="23">
+        <v>747</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G11" t="s">
         <v>40</v>
       </c>
-      <c r="H10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" t="s">
-        <v>116</v>
-      </c>
-      <c r="J10" s="13">
-        <v>0.99</v>
-      </c>
-      <c r="K10" s="13">
-        <v>1.19</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="6">
-        <v>128</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" t="s">
+        <v>173</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="L11" s="25" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="6">
+        <v>149</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="6">
+        <v>134</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="D13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="F13" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12">
-        <v>1379</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" t="s">
-        <v>118</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="6">
-        <v>203</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>27</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="J13" s="12">
-        <v>5</v>
-      </c>
-      <c r="K13" s="12" t="s">
+        <v>8.9</v>
+      </c>
+      <c r="K13" s="12">
+        <v>6</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="23">
+        <v>156</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" t="s">
+        <v>158</v>
+      </c>
+      <c r="I14" t="s">
+        <v>159</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="L14" s="25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15">
+        <v>262</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" t="s">
+        <v>114</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0.99</v>
+      </c>
+      <c r="K15" s="13">
+        <v>1.19</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="6">
+        <v>128</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="L13" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="9" t="s">
+      <c r="M16" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17">
+        <v>1379</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="G14" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" t="s">
-        <v>119</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="L14" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15">
-        <v>216</v>
-      </c>
-      <c r="C15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" t="s">
-        <v>93</v>
-      </c>
-      <c r="I15" t="s">
-        <v>120</v>
-      </c>
-      <c r="J15" s="16">
-        <v>3.4</v>
-      </c>
-      <c r="K15" s="16">
-        <v>1.99</v>
-      </c>
-      <c r="L15" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B16">
-        <v>996</v>
-      </c>
-      <c r="C16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" t="s">
-        <v>169</v>
-      </c>
-      <c r="E16" t="s">
-        <v>133</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="H16" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" t="s">
-        <v>136</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>139</v>
-      </c>
-      <c r="B17">
-        <v>105</v>
-      </c>
-      <c r="C17" t="s">
-        <v>142</v>
-      </c>
-      <c r="D17" t="s">
-        <v>141</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>172</v>
       </c>
       <c r="G17" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>170</v>
+      <c r="H17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>116</v>
       </c>
       <c r="J17" s="13" t="s">
         <v>70</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>147</v>
-      </c>
-      <c r="B18" s="23">
-        <v>110</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="E18" t="s">
-        <v>149</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="G18" t="s">
-        <v>135</v>
-      </c>
-      <c r="H18" t="s">
-        <v>134</v>
-      </c>
-      <c r="I18" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="K18" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="L18" s="25" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="6">
+        <v>203</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="12">
+        <v>5</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>181</v>
-      </c>
-      <c r="B19" s="23">
-        <v>747</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>151</v>
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>153</v>
+        <v>18</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>160</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H19" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="I19" t="s">
-        <v>179</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="K19" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="L19" s="25" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="L19" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>166</v>
-      </c>
-      <c r="B20" s="23">
-        <v>156</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>156</v>
+        <v>61</v>
+      </c>
+      <c r="B20">
+        <v>216</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>157</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>159</v>
+        <v>31</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>161</v>
+        <v>24</v>
       </c>
       <c r="G20" t="s">
-        <v>162</v>
+        <v>44</v>
       </c>
       <c r="H20" t="s">
-        <v>163</v>
+        <v>92</v>
       </c>
       <c r="I20" t="s">
-        <v>164</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="L20" s="25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+      <c r="J20" s="16">
+        <v>3.4</v>
+      </c>
+      <c r="K20" s="16">
+        <v>1.99</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B21">
         <f>SUBTOTAL(109,Tabelle3[Sample size])</f>
         <v>5699</v>
@@ -2184,43 +2194,43 @@
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="F22" s="9"/>
       <c r="L22" s="15"/>
     </row>
-    <row r="23" spans="1:12" ht="409.6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="6.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="C24" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E25" s="2"/>
       <c r="F25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E31" s="2"/>
       <c r="H31" t="s">
         <v>22</v>
@@ -2249,8 +2259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2267,144 +2277,144 @@
         <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>68</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>69</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="21">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="D2">
-        <v>0.09</v>
-      </c>
-      <c r="E2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="21">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="I2">
-        <v>0.33</v>
-      </c>
-      <c r="J2" t="s">
-        <v>187</v>
+      <c r="A2" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="23">
+        <v>0.16</v>
+      </c>
+      <c r="C2" s="23">
+        <v>0.06</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
-        <v>181</v>
+        <v>137</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="D3" s="27">
-        <v>0.13</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>185</v>
+        <v>70</v>
+      </c>
+      <c r="C3" s="23">
+        <v>3.1</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>179</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>188</v>
+        <v>25</v>
       </c>
       <c r="G3" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="23">
-        <v>5.53</v>
+      <c r="H3" s="26">
+        <v>5.2</v>
       </c>
       <c r="I3" s="23">
-        <v>0.33</v>
+        <v>0.41</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>70</v>
       </c>
       <c r="C4">
-        <v>2.1</v>
-      </c>
-      <c r="D4">
-        <v>0.16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>189</v>
+        <v>4.93</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.37</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" t="s">
-        <v>70</v>
+      <c r="H4" s="5">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="I4">
+        <v>0.66</v>
       </c>
       <c r="J4" t="s">
-        <v>70</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>70</v>
       </c>
       <c r="C5">
-        <v>2.81</v>
+        <v>1.6</v>
       </c>
       <c r="D5">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="E5" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="F5" t="s">
         <v>25</v>
@@ -2413,414 +2423,414 @@
         <v>70</v>
       </c>
       <c r="H5" s="5">
-        <v>2.27</v>
+        <v>2.6</v>
       </c>
       <c r="I5">
-        <v>0.17</v>
+        <v>0.37</v>
       </c>
       <c r="J5" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>70</v>
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>2.4900000000000002</v>
       </c>
       <c r="C6">
-        <v>1.6</v>
+        <v>3.03</v>
       </c>
       <c r="D6">
-        <v>0.21</v>
+        <v>0.4</v>
       </c>
       <c r="E6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="G6" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="5">
-        <v>2.6</v>
-      </c>
-      <c r="I6">
-        <v>0.37</v>
+      <c r="H6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" t="s">
+        <v>70</v>
       </c>
       <c r="J6" t="s">
-        <v>187</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="23">
-        <v>0.22</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="23">
-        <v>0.46</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>187</v>
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>4.2</v>
+      </c>
+      <c r="C7">
+        <v>1.78</v>
+      </c>
+      <c r="D7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="5">
+        <v>3.58</v>
+      </c>
+      <c r="I7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J7" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>70</v>
       </c>
       <c r="C8">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D8">
-        <v>0.24</v>
+        <v>1.35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>189</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="G8" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="5">
-        <v>6.13</v>
-      </c>
-      <c r="I8">
-        <v>0.65</v>
+      <c r="H8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" t="s">
+        <v>70</v>
       </c>
       <c r="J8" t="s">
-        <v>190</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="23">
-        <v>3.1</v>
-      </c>
-      <c r="D9" s="23">
-        <v>0.25</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="26">
-        <v>5.2</v>
-      </c>
-      <c r="I9" s="23">
-        <v>0.41</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>185</v>
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9">
+        <v>2.33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10">
-        <v>3.25</v>
-      </c>
-      <c r="D10">
-        <v>0.27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>189</v>
-      </c>
-      <c r="F10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="A10" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="23">
+        <v>0.35</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="23" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="D11">
-        <v>0.27800000000000002</v>
-      </c>
-      <c r="E11" t="s">
-        <v>190</v>
-      </c>
-      <c r="F11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J11" t="s">
-        <v>70</v>
+      <c r="A11" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="23">
+        <v>0.54</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="23">
+        <v>1.17</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12">
-        <v>4.2</v>
-      </c>
-      <c r="C12">
-        <v>1.78</v>
-      </c>
-      <c r="D12">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E12" t="s">
-        <v>185</v>
-      </c>
-      <c r="F12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="5">
-        <v>3.58</v>
-      </c>
-      <c r="I12">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="J12" t="s">
-        <v>187</v>
+      <c r="A12" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D12" s="27">
+        <v>0.13</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="23">
+        <v>5.53</v>
+      </c>
+      <c r="I12" s="23">
+        <v>0.33</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13">
-        <v>3.4</v>
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
       </c>
       <c r="C13">
-        <v>1.99</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="D13">
-        <v>0.28999999999999998</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E13" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
         <v>70</v>
       </c>
-      <c r="H13" s="5">
-        <v>4.5599999999999996</v>
-      </c>
-      <c r="I13">
-        <v>0.7</v>
+      <c r="H13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" t="s">
+        <v>70</v>
       </c>
       <c r="J13" t="s">
-        <v>190</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="23">
-        <v>0.35</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="J14" s="23" t="s">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="D14">
+        <v>0.47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>181</v>
+      </c>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="23">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15">
+        <v>8.9</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>0.51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="23">
         <v>0.36</v>
       </c>
-      <c r="E15" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="F15" s="23" t="s">
+      <c r="E16" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="F16" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="I15" s="23">
+      <c r="G16" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" s="23">
         <v>0.61</v>
       </c>
-      <c r="J15" s="23" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16">
-        <v>4.93</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.37</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="5">
-        <v>9.0500000000000007</v>
-      </c>
-      <c r="I16">
-        <v>0.66</v>
-      </c>
-      <c r="J16" t="s">
-        <v>187</v>
+      <c r="J16" s="23" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="C17">
-        <v>3.03</v>
-      </c>
-      <c r="D17">
-        <v>0.4</v>
-      </c>
-      <c r="E17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F17" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" t="s">
-        <v>70</v>
-      </c>
-      <c r="J17" t="s">
-        <v>70</v>
+      <c r="A17" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="23">
+        <v>0.22</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="I17" s="23">
+        <v>0.46</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" t="s">
-        <v>70</v>
+        <v>57</v>
+      </c>
+      <c r="B18">
+        <v>0.99</v>
       </c>
       <c r="C18">
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="D18">
-        <v>0.47</v>
+        <v>1.19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
       </c>
       <c r="E18" t="s">
-        <v>187</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
         <v>70</v>
@@ -2840,83 +2850,83 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19">
-        <v>8.9</v>
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D19">
-        <v>0.51</v>
+        <v>0.24</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>183</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="G19" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I19" t="s">
-        <v>70</v>
+      <c r="H19" s="5">
+        <v>6.13</v>
+      </c>
+      <c r="I19">
+        <v>0.65</v>
       </c>
       <c r="J19" t="s">
-        <v>70</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="23">
-        <v>0.54</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I20" s="23">
-        <v>1.17</v>
-      </c>
-      <c r="J20" s="23" t="s">
-        <v>187</v>
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="21">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.09</v>
+      </c>
+      <c r="E20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
+        <v>70</v>
+      </c>
+      <c r="H20" s="21">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="I20">
+        <v>0.33</v>
+      </c>
+      <c r="J20" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" t="s">
-        <v>70</v>
+        <v>60</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>4.0199999999999996</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="D21">
-        <v>0.55000000000000004</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="E21" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F21" t="s">
         <v>70</v>
@@ -2936,19 +2946,19 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
         <v>70</v>
       </c>
       <c r="C22">
-        <v>6.53</v>
+        <v>2.81</v>
       </c>
       <c r="D22">
-        <v>0.56999999999999995</v>
+        <v>0.2</v>
       </c>
       <c r="E22" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="F22" t="s">
         <v>25</v>
@@ -2957,94 +2967,94 @@
         <v>70</v>
       </c>
       <c r="H22" s="5">
-        <v>8.07</v>
+        <v>2.27</v>
       </c>
       <c r="I22">
-        <v>0.71</v>
+        <v>0.17</v>
       </c>
       <c r="J22" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B23" s="23">
-        <v>0.16</v>
-      </c>
-      <c r="C23" s="23">
-        <v>0.06</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="J23" s="23" t="s">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23">
+        <v>3.25</v>
+      </c>
+      <c r="D23">
+        <v>0.27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>183</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
         <v>70</v>
       </c>
       <c r="C24">
-        <v>1.35</v>
-      </c>
-      <c r="D24" t="s">
-        <v>70</v>
+        <v>6.53</v>
+      </c>
+      <c r="D24">
+        <v>0.56999999999999995</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>184</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="G24" t="s">
         <v>70</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I24" t="s">
-        <v>70</v>
+      <c r="H24" s="5">
+        <v>8.07</v>
+      </c>
+      <c r="I24">
+        <v>0.71</v>
       </c>
       <c r="J24" t="s">
-        <v>70</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>70</v>
       </c>
       <c r="C25">
-        <v>2.33</v>
-      </c>
-      <c r="D25" t="s">
-        <v>70</v>
+        <v>2.1</v>
+      </c>
+      <c r="D25">
+        <v>0.16</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>183</v>
       </c>
       <c r="F25" t="s">
         <v>70</v>
@@ -3064,34 +3074,34 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B26">
-        <v>0.99</v>
+        <v>3.4</v>
       </c>
       <c r="C26">
-        <v>1.19</v>
-      </c>
-      <c r="D26" t="s">
-        <v>70</v>
+        <v>1.99</v>
+      </c>
+      <c r="D26">
+        <v>0.28999999999999998</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>184</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="G26" t="s">
         <v>70</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I26" t="s">
-        <v>70</v>
+      <c r="H26" s="5">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="I26">
+        <v>0.7</v>
       </c>
       <c r="J26" t="s">
-        <v>70</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -3130,31 +3140,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>87</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
         <v>88</v>
       </c>
-      <c r="F1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" t="s">
-        <v>89</v>
-      </c>
       <c r="I1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -3188,7 +3198,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3">
         <v>7.01</v>
@@ -3242,7 +3252,7 @@
         <v>70</v>
       </c>
       <c r="I4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>